<commit_message>
Updated User Stories, Old folders deleted, Test Cases
</commit_message>
<xml_diff>
--- a/6K185_DocShare_DayCare/Iteration1_10-10/NEWUpdated of Daycare_UserStories.xlsx
+++ b/6K185_DocShare_DayCare/Iteration1_10-10/NEWUpdated of Daycare_UserStories.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="496" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="496"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="6" r:id="rId1"/>
-    <sheet name="StoriesDetailsIteration1" sheetId="7" r:id="rId2"/>
-    <sheet name="Cover Sheet" sheetId="3" r:id="rId3"/>
-    <sheet name="Actors" sheetId="4" r:id="rId4"/>
+    <sheet name="TestCases" sheetId="8" r:id="rId2"/>
+    <sheet name="StoriesDetailsIteration1" sheetId="7" r:id="rId3"/>
+    <sheet name="Cover Sheet" sheetId="3" r:id="rId4"/>
+    <sheet name="Actors" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -282,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="171">
   <si>
     <t>Story ID</t>
   </si>
@@ -494,9 +495,6 @@
     <t xml:space="preserve">Maintain Contact Information/ Emergency </t>
   </si>
   <si>
-    <t>Maintain own hours</t>
-  </si>
-  <si>
     <t>Check In / Check Out Kids</t>
   </si>
   <si>
@@ -623,9 +621,6 @@
     <t>Accident Types</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>Event Calendar Update</t>
   </si>
   <si>
@@ -804,13 +799,76 @@
   </si>
   <si>
     <t>S104.vis</t>
+  </si>
+  <si>
+    <t>Working?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Works/ contact info still needs to be added</t>
+  </si>
+  <si>
+    <t>Error exception handling not implemented yet</t>
+  </si>
+  <si>
+    <t>Works</t>
+  </si>
+  <si>
+    <t>Works / Picture displays needs to be edited for internal logins (Admins/ Teachers)</t>
+  </si>
+  <si>
+    <t>Ggl Cal not implemented yet</t>
+  </si>
+  <si>
+    <t>Works / More users for tests still need to be added here!</t>
+  </si>
+  <si>
+    <t>Works? Logout not tested yet!</t>
+  </si>
+  <si>
+    <t>Not completed --&gt; No DB connection , no tests</t>
+  </si>
+  <si>
+    <t>Current Developers:</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Waleed</t>
+  </si>
+  <si>
+    <t>Iteration 3</t>
+  </si>
+  <si>
+    <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Wyatt</t>
+  </si>
+  <si>
+    <t>Test Cases Iteration 1</t>
+  </si>
+  <si>
+    <t>IN PROGRESS!</t>
+  </si>
+  <si>
+    <t>David</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,8 +925,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,6 +958,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +1018,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -972,6 +1070,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1294,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,9 +1420,11 @@
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="50.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1324,19 +1440,28 @@
       <c r="E1" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>2</v>
@@ -1348,12 +1473,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>2</v>
@@ -1365,108 +1490,151 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="E5" s="21">
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G6" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="22">
+        <v>3</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="14" t="s">
         <v>4</v>
@@ -1474,39 +1642,48 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13">
+        <v>62</v>
+      </c>
+      <c r="E13" s="22">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G13" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -1517,13 +1694,19 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -1531,19 +1714,28 @@
       <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="E17">
-        <v>1</v>
+      <c r="E17" s="22">
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1555,12 +1747,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1572,38 +1764,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
@@ -1614,30 +1806,45 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>45</v>
@@ -1645,19 +1852,28 @@
       <c r="D25" t="s">
         <v>37</v>
       </c>
-      <c r="E25">
-        <v>1</v>
+      <c r="E25" s="22">
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>45</v>
@@ -1669,12 +1885,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
         <v>45</v>
@@ -1686,160 +1902,184 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
         <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="E28" s="22">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
-      <c r="B32" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>41</v>
@@ -1850,10 +2090,16 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B39" t="s">
         <v>99</v>
@@ -1861,28 +2107,38 @@
       <c r="C39" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="8" t="s">
         <v>80</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B42" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1898,11 +2154,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,7 +2180,7 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="38.140625" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1930,94 +2198,94 @@
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I4" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>145</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J5" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2034,47 +2302,47 @@
     </row>
     <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J7" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -2084,41 +2352,41 @@
     </row>
     <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>2</v>
@@ -2127,16 +2395,16 @@
         <v>33</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2146,10 +2414,10 @@
     </row>
     <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>35</v>
@@ -2158,14 +2426,14 @@
         <v>36</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -2173,10 +2441,10 @@
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>35</v>
@@ -2187,10 +2455,10 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -2249,10 +2517,10 @@
     </row>
     <row r="20" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>45</v>
@@ -2261,14 +2529,14 @@
         <v>39</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -2276,24 +2544,24 @@
     </row>
     <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -2301,10 +2569,10 @@
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>45</v>
@@ -2315,15 +2583,15 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2382,10 +2650,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>41</v>
@@ -2394,7 +2662,7 @@
         <v>42</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -2405,16 +2673,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
@@ -2426,16 +2694,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
@@ -2447,16 +2715,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
@@ -2468,16 +2736,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
@@ -2489,16 +2757,16 @@
     </row>
     <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
@@ -2514,7 +2782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -2630,7 +2898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2671,10 +2939,10 @@
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2682,7 +2950,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">

</xml_diff>